<commit_message>
Updated Dyno Electrical System Diagram to V1.2
Created Dyno Electrical System Diagram V2.0
***Important Note: This does not obsolete V1.2, both will be used in separate test conditions.  V2.0 adds CAN Mirror into Dyno configuration.
</commit_message>
<xml_diff>
--- a/RW-3 Connector Master List.xlsx
+++ b/RW-3 Connector Master List.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="195">
   <si>
     <t>Connector Number</t>
   </si>
@@ -619,6 +619,27 @@
   </si>
   <si>
     <t>CAN A to Motor Controller (dyno)</t>
+  </si>
+  <si>
+    <t>X-1001</t>
+  </si>
+  <si>
+    <t>X-1002</t>
+  </si>
+  <si>
+    <t>2-crkt MX-150L</t>
+  </si>
+  <si>
+    <t>C-1004</t>
+  </si>
+  <si>
+    <t>C-1005</t>
+  </si>
+  <si>
+    <t>CAN A from Dyno CAN Backplane to Tritium</t>
+  </si>
+  <si>
+    <t>Short CAN to CAN jumper</t>
   </si>
 </sst>
 </file>
@@ -810,11 +831,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -846,11 +873,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1183,11 +1207,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,19 +1245,19 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="H2" s="4" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="H2" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="6"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1248,9 +1272,9 @@
       <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="11"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1265,9 +1289,9 @@
       <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="11"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1282,9 +1306,9 @@
       <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="11"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1299,51 +1323,54 @@
       <c r="E6" t="s">
         <v>141</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="14"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" t="s">
+        <v>141</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s">
-        <v>23</v>
-      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>26</v>
@@ -1352,26 +1379,26 @@
         <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
@@ -1380,23 +1407,26 @@
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
@@ -1405,12 +1435,12 @@
         <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
         <v>26</v>
@@ -1419,89 +1449,86 @@
         <v>20</v>
       </c>
     </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" t="s">
-        <v>22</v>
-      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
         <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
         <v>20</v>
       </c>
       <c r="E23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
         <v>47</v>
@@ -1510,12 +1537,12 @@
         <v>20</v>
       </c>
       <c r="E24" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
         <v>45</v>
@@ -1524,26 +1551,26 @@
         <v>20</v>
       </c>
       <c r="E25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
         <v>20</v>
       </c>
       <c r="E26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
         <v>45</v>
@@ -1552,40 +1579,40 @@
         <v>20</v>
       </c>
       <c r="E27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
         <v>20</v>
       </c>
       <c r="E28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C29" t="s">
         <v>20</v>
       </c>
       <c r="E29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B30" t="s">
         <v>47</v>
@@ -1594,54 +1621,54 @@
         <v>20</v>
       </c>
       <c r="E30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="E31" t="s">
-        <v>108</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C32" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="E32" t="s">
-        <v>109</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s">
         <v>107</v>
       </c>
       <c r="E33" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B34" t="s">
         <v>50</v>
@@ -1650,12 +1677,12 @@
         <v>107</v>
       </c>
       <c r="E34" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B35" t="s">
         <v>50</v>
@@ -1664,12 +1691,12 @@
         <v>107</v>
       </c>
       <c r="E35" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B36" t="s">
         <v>50</v>
@@ -1678,12 +1705,12 @@
         <v>107</v>
       </c>
       <c r="E36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B37" t="s">
         <v>50</v>
@@ -1692,12 +1719,12 @@
         <v>107</v>
       </c>
       <c r="E37" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B38" t="s">
         <v>50</v>
@@ -1706,12 +1733,12 @@
         <v>107</v>
       </c>
       <c r="E38" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B39" t="s">
         <v>50</v>
@@ -1720,12 +1747,12 @@
         <v>107</v>
       </c>
       <c r="E39" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B40" t="s">
         <v>50</v>
@@ -1734,12 +1761,12 @@
         <v>107</v>
       </c>
       <c r="E40" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B41" t="s">
         <v>50</v>
@@ -1748,12 +1775,12 @@
         <v>107</v>
       </c>
       <c r="E41" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B42" t="s">
         <v>50</v>
@@ -1762,12 +1789,12 @@
         <v>107</v>
       </c>
       <c r="E42" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B43" t="s">
         <v>50</v>
@@ -1776,12 +1803,12 @@
         <v>107</v>
       </c>
       <c r="E43" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B44" t="s">
         <v>50</v>
@@ -1790,12 +1817,12 @@
         <v>107</v>
       </c>
       <c r="E44" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B45" t="s">
         <v>50</v>
@@ -1804,12 +1831,12 @@
         <v>107</v>
       </c>
       <c r="E45" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B46" t="s">
         <v>50</v>
@@ -1818,90 +1845,90 @@
         <v>107</v>
       </c>
       <c r="E46" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C47" t="s">
         <v>107</v>
       </c>
+      <c r="E47" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>42</v>
+        <v>105</v>
       </c>
       <c r="B48" t="s">
         <v>50</v>
       </c>
       <c r="C48" t="s">
-        <v>20</v>
+        <v>107</v>
+      </c>
+      <c r="E48" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="B49" t="s">
-        <v>169</v>
+        <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>20</v>
-      </c>
-      <c r="E49" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B50" t="s">
-        <v>169</v>
+        <v>50</v>
       </c>
       <c r="C50" t="s">
         <v>20</v>
-      </c>
-      <c r="E50" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>136</v>
+        <v>43</v>
       </c>
       <c r="B51" t="s">
-        <v>50</v>
+        <v>169</v>
       </c>
       <c r="C51" t="s">
-        <v>132</v>
+        <v>20</v>
       </c>
       <c r="E51" t="s">
-        <v>140</v>
+        <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>137</v>
+        <v>44</v>
       </c>
       <c r="B52" t="s">
-        <v>50</v>
+        <v>169</v>
       </c>
       <c r="C52" t="s">
-        <v>132</v>
+        <v>20</v>
       </c>
       <c r="E52" t="s">
-        <v>139</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B53" t="s">
         <v>50</v>
@@ -1913,61 +1940,61 @@
         <v>140</v>
       </c>
     </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>137</v>
+      </c>
+      <c r="B54" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" t="s">
+        <v>132</v>
+      </c>
+      <c r="E54" t="s">
+        <v>139</v>
+      </c>
+    </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+      <c r="A55" t="s">
+        <v>138</v>
+      </c>
+      <c r="B55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" t="s">
+        <v>132</v>
+      </c>
+      <c r="E55" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>56</v>
-      </c>
-      <c r="B56" t="s">
-        <v>68</v>
-      </c>
-      <c r="C56" t="s">
-        <v>20</v>
-      </c>
-      <c r="E56" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>57</v>
-      </c>
-      <c r="B57" t="s">
-        <v>68</v>
-      </c>
-      <c r="C57" t="s">
-        <v>20</v>
-      </c>
-      <c r="E57" t="s">
-        <v>48</v>
-      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C58" t="s">
         <v>20</v>
       </c>
       <c r="E58" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B59" t="s">
         <v>68</v>
@@ -1976,76 +2003,76 @@
         <v>20</v>
       </c>
       <c r="E59" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C60" t="s">
         <v>20</v>
       </c>
       <c r="E60" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C61" t="s">
         <v>20</v>
+      </c>
+      <c r="E61" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C62" t="s">
         <v>20</v>
+      </c>
+      <c r="E62" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C63" t="s">
         <v>20</v>
-      </c>
-      <c r="E63" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C64" t="s">
         <v>20</v>
-      </c>
-      <c r="E64" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B65" t="s">
         <v>70</v>
@@ -2054,12 +2081,12 @@
         <v>20</v>
       </c>
       <c r="E65" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B66" t="s">
         <v>70</v>
@@ -2067,198 +2094,204 @@
       <c r="C66" t="s">
         <v>20</v>
       </c>
+      <c r="E66" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C67" t="s">
         <v>20</v>
+      </c>
+      <c r="E67" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>133</v>
+        <v>66</v>
       </c>
       <c r="B68" t="s">
         <v>70</v>
       </c>
       <c r="C68" t="s">
-        <v>132</v>
-      </c>
-      <c r="E68" t="s">
-        <v>142</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>71</v>
+      </c>
+      <c r="C69" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>133</v>
+      </c>
+      <c r="B70" t="s">
+        <v>70</v>
+      </c>
+      <c r="C70" t="s">
+        <v>132</v>
+      </c>
+      <c r="E70" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>134</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B71" t="s">
         <v>70</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C71" t="s">
         <v>132</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E71" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>74</v>
-      </c>
-      <c r="B72" t="s">
-        <v>84</v>
-      </c>
-      <c r="C72" t="s">
-        <v>20</v>
-      </c>
-      <c r="E72" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>75</v>
-      </c>
-      <c r="B73" t="s">
-        <v>85</v>
-      </c>
-      <c r="C73" t="s">
-        <v>20</v>
-      </c>
-      <c r="E73" t="s">
-        <v>48</v>
-      </c>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C74" t="s">
         <v>20</v>
       </c>
       <c r="E74" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C75" t="s">
         <v>20</v>
       </c>
       <c r="E75" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C76" t="s">
         <v>20</v>
+      </c>
+      <c r="E76" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>118</v>
+        <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>125</v>
+        <v>86</v>
       </c>
       <c r="C77" t="s">
-        <v>107</v>
+        <v>20</v>
+      </c>
+      <c r="E77" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>119</v>
+        <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>125</v>
+        <v>87</v>
       </c>
       <c r="C78" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B79" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C79" t="s">
         <v>107</v>
       </c>
-      <c r="E79" t="s">
-        <v>127</v>
-      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B80" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C80" t="s">
         <v>107</v>
       </c>
-      <c r="E80" t="s">
-        <v>129</v>
-      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B81" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C81" t="s">
         <v>107</v>
       </c>
+      <c r="E81" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B82" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C82" t="s">
         <v>107</v>
       </c>
+      <c r="E82" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B83" t="s">
         <v>130</v>
@@ -2269,84 +2302,106 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="B84" t="s">
-        <v>86</v>
+        <v>130</v>
       </c>
       <c r="C84" t="s">
-        <v>132</v>
-      </c>
-      <c r="E84" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>124</v>
+      </c>
+      <c r="B85" t="s">
+        <v>130</v>
+      </c>
+      <c r="C85" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>144</v>
+      </c>
+      <c r="B86" t="s">
+        <v>86</v>
+      </c>
+      <c r="C86" t="s">
+        <v>132</v>
+      </c>
+      <c r="E86" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>143</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B87" t="s">
         <v>86</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C87" t="s">
         <v>132</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E87" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>80</v>
-      </c>
-      <c r="B88" t="s">
-        <v>88</v>
-      </c>
-      <c r="C88" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>81</v>
-      </c>
-      <c r="B89" t="s">
-        <v>88</v>
-      </c>
-      <c r="C89" t="s">
-        <v>20</v>
-      </c>
+      <c r="B89" s="5"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>80</v>
+      </c>
+      <c r="B90" t="s">
+        <v>88</v>
+      </c>
+      <c r="C90" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>81</v>
+      </c>
+      <c r="B91" t="s">
+        <v>88</v>
+      </c>
+      <c r="C91" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>82</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B92" t="s">
         <v>89</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C92" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A73:F73"/>
+    <mergeCell ref="A89:F89"/>
     <mergeCell ref="H2:J6"/>
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="A71:F71"/>
-    <mergeCell ref="A87:F87"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A57:F57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2355,10 +2410,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G39" sqref="G38:G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2368,7 +2423,7 @@
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20" style="14" customWidth="1"/>
+    <col min="6" max="6" width="20" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2387,7 +2442,7 @@
       <c r="E1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="3" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2398,14 +2453,14 @@
       <c r="B2">
         <v>5</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="18"/>
     </row>
     <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2414,12 +2469,12 @@
       <c r="B3">
         <v>6</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="20"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2428,12 +2483,12 @@
       <c r="B4">
         <v>6</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="23"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -2442,7 +2497,7 @@
       <c r="B5">
         <v>8</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="4" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2453,7 +2508,7 @@
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="4" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2464,7 +2519,7 @@
       <c r="B7">
         <v>7</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="4" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2475,7 +2530,7 @@
       <c r="B8">
         <v>8</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="4" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2486,7 +2541,7 @@
       <c r="B9">
         <v>3</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="4" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2497,7 +2552,7 @@
       <c r="B10">
         <v>3</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="4" t="s">
         <v>161</v>
       </c>
     </row>
@@ -2508,7 +2563,7 @@
       <c r="B11">
         <v>3</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="4" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2522,7 +2577,7 @@
       <c r="E12" t="s">
         <v>166</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="4" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2536,7 +2591,7 @@
       <c r="E13" t="s">
         <v>166</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="4" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2550,7 +2605,7 @@
       <c r="E14" t="s">
         <v>166</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="4" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2564,7 +2619,7 @@
       <c r="E15" t="s">
         <v>166</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="4" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2578,7 +2633,7 @@
       <c r="E16" t="s">
         <v>166</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="4" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2589,7 +2644,7 @@
       <c r="B17">
         <v>6</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="4" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2600,7 +2655,7 @@
       <c r="B18">
         <v>6</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="4" t="s">
         <v>171</v>
       </c>
     </row>
@@ -2611,7 +2666,7 @@
       <c r="B19">
         <v>6</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="4" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2622,7 +2677,7 @@
       <c r="B20">
         <v>6</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="4" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2633,7 +2688,7 @@
       <c r="B21">
         <v>6</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="4" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2644,7 +2699,7 @@
       <c r="B22">
         <v>6</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="4" t="s">
         <v>175</v>
       </c>
     </row>
@@ -2655,7 +2710,7 @@
       <c r="B23">
         <v>6</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="4" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2666,7 +2721,7 @@
       <c r="B24">
         <v>6</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="4" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2677,7 +2732,7 @@
       <c r="B25">
         <v>6</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="4" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2688,7 +2743,7 @@
       <c r="B26">
         <v>3</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="4" t="s">
         <v>178</v>
       </c>
     </row>
@@ -2699,7 +2754,7 @@
       <c r="B27">
         <v>2</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="4" t="s">
         <v>179</v>
       </c>
     </row>
@@ -2710,7 +2765,7 @@
       <c r="B28" t="s">
         <v>182</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="4" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2721,7 +2776,7 @@
       <c r="B29" t="s">
         <v>182</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="4" t="s">
         <v>181</v>
       </c>
     </row>
@@ -2732,7 +2787,7 @@
       <c r="B31">
         <v>3</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="4" t="s">
         <v>184</v>
       </c>
     </row>
@@ -2743,7 +2798,7 @@
       <c r="B32">
         <v>4</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="4" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2754,7 +2809,7 @@
       <c r="B33">
         <v>6</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F33" s="4" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2765,8 +2820,30 @@
       <c r="B34">
         <v>6</v>
       </c>
-      <c r="F34" s="14" t="s">
+      <c r="F34" s="4" t="s">
         <v>187</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>191</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>192</v>
+      </c>
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made progress on Rear Enclosure Diagram
</commit_message>
<xml_diff>
--- a/RW-3 Connector Master List.xlsx
+++ b/RW-3 Connector Master List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="208">
   <si>
     <t>Connector Number</t>
   </si>
@@ -640,6 +640,45 @@
   </si>
   <si>
     <t>Short CAN to CAN jumper</t>
+  </si>
+  <si>
+    <t>C-128</t>
+  </si>
+  <si>
+    <t>Contactor Logic to 12V Terminal Block &amp; X-101</t>
+  </si>
+  <si>
+    <t>X-512</t>
+  </si>
+  <si>
+    <t>x-513</t>
+  </si>
+  <si>
+    <t>X-514</t>
+  </si>
+  <si>
+    <t>X-515</t>
+  </si>
+  <si>
+    <t>X-516</t>
+  </si>
+  <si>
+    <t>2-crkt Duraclik</t>
+  </si>
+  <si>
+    <t>2-crkt Mate-N-Lok</t>
+  </si>
+  <si>
+    <t>8-crkt Mate-N-Lok</t>
+  </si>
+  <si>
+    <t>Rear Enclosure Diagram</t>
+  </si>
+  <si>
+    <t>C-129</t>
+  </si>
+  <si>
+    <t>X-333</t>
   </si>
 </sst>
 </file>
@@ -1207,11 +1246,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:J98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1928,21 +1967,21 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>136</v>
+        <v>207</v>
       </c>
       <c r="B53" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C53" t="s">
-        <v>132</v>
+        <v>205</v>
       </c>
       <c r="E53" t="s">
-        <v>140</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B54" t="s">
         <v>50</v>
@@ -1951,12 +1990,12 @@
         <v>132</v>
       </c>
       <c r="E54" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B55" t="s">
         <v>50</v>
@@ -1965,36 +2004,36 @@
         <v>132</v>
       </c>
       <c r="E55" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>138</v>
+      </c>
+      <c r="B56" t="s">
+        <v>50</v>
+      </c>
+      <c r="C56" t="s">
+        <v>132</v>
+      </c>
+      <c r="E56" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>56</v>
-      </c>
-      <c r="B58" t="s">
-        <v>68</v>
-      </c>
-      <c r="C58" t="s">
-        <v>20</v>
-      </c>
-      <c r="E58" t="s">
-        <v>46</v>
-      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" t="s">
         <v>68</v>
@@ -2003,40 +2042,40 @@
         <v>20</v>
       </c>
       <c r="E59" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C60" t="s">
         <v>20</v>
       </c>
       <c r="E60" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C61" t="s">
         <v>20</v>
       </c>
       <c r="E61" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" t="s">
         <v>68</v>
@@ -2045,23 +2084,26 @@
         <v>20</v>
       </c>
       <c r="E62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C63" t="s">
         <v>20</v>
+      </c>
+      <c r="E63" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" t="s">
         <v>69</v>
@@ -2072,21 +2114,18 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C65" t="s">
         <v>20</v>
-      </c>
-      <c r="E65" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66" t="s">
         <v>70</v>
@@ -2095,12 +2134,12 @@
         <v>20</v>
       </c>
       <c r="E66" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67" t="s">
         <v>70</v>
@@ -2109,12 +2148,12 @@
         <v>20</v>
       </c>
       <c r="E67" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68" t="s">
         <v>70</v>
@@ -2122,13 +2161,16 @@
       <c r="C68" t="s">
         <v>20</v>
       </c>
+      <c r="E68" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C69" t="s">
         <v>20</v>
@@ -2136,21 +2178,18 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>133</v>
+        <v>67</v>
       </c>
       <c r="B70" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C70" t="s">
-        <v>132</v>
-      </c>
-      <c r="E70" t="s">
-        <v>142</v>
+        <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B71" t="s">
         <v>70</v>
@@ -2162,50 +2201,50 @@
         <v>142</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>134</v>
+      </c>
+      <c r="B72" t="s">
+        <v>70</v>
+      </c>
+      <c r="C72" t="s">
+        <v>132</v>
+      </c>
+      <c r="E72" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>74</v>
-      </c>
-      <c r="B74" t="s">
-        <v>84</v>
-      </c>
-      <c r="C74" t="s">
-        <v>20</v>
-      </c>
-      <c r="E74" t="s">
-        <v>22</v>
-      </c>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C75" t="s">
         <v>20</v>
       </c>
       <c r="E75" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C76" t="s">
         <v>20</v>
@@ -2216,7 +2255,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B77" t="s">
         <v>86</v>
@@ -2225,34 +2264,37 @@
         <v>20</v>
       </c>
       <c r="E77" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C78" t="s">
         <v>20</v>
+      </c>
+      <c r="E78" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>125</v>
+        <v>87</v>
       </c>
       <c r="C79" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B80" t="s">
         <v>125</v>
@@ -2263,46 +2305,46 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B81" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C81" t="s">
         <v>107</v>
       </c>
-      <c r="E81" t="s">
-        <v>127</v>
-      </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B82" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C82" t="s">
         <v>107</v>
       </c>
       <c r="E82" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B83" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C83" t="s">
         <v>107</v>
       </c>
+      <c r="E83" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B84" t="s">
         <v>130</v>
@@ -2313,7 +2355,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B85" t="s">
         <v>130</v>
@@ -2324,84 +2366,153 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="B86" t="s">
-        <v>86</v>
+        <v>130</v>
       </c>
       <c r="C86" t="s">
-        <v>132</v>
-      </c>
-      <c r="E86" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>143</v>
+        <v>197</v>
       </c>
       <c r="B87" t="s">
-        <v>86</v>
+        <v>202</v>
       </c>
       <c r="C87" t="s">
-        <v>132</v>
-      </c>
-      <c r="E87" t="s">
-        <v>142</v>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>198</v>
+      </c>
+      <c r="B88" t="s">
+        <v>202</v>
+      </c>
+      <c r="C88" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
+      <c r="A89" t="s">
+        <v>199</v>
+      </c>
+      <c r="B89" t="s">
+        <v>203</v>
+      </c>
+      <c r="C89" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="B90" t="s">
-        <v>88</v>
+        <v>203</v>
       </c>
       <c r="C90" t="s">
-        <v>20</v>
+        <v>205</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>81</v>
+        <v>201</v>
       </c>
       <c r="B91" t="s">
-        <v>88</v>
+        <v>204</v>
       </c>
       <c r="C91" t="s">
-        <v>20</v>
+        <v>205</v>
+      </c>
+      <c r="E91" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>144</v>
+      </c>
+      <c r="B92" t="s">
+        <v>86</v>
+      </c>
+      <c r="C92" t="s">
+        <v>132</v>
+      </c>
+      <c r="E92" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>143</v>
+      </c>
+      <c r="B93" t="s">
+        <v>86</v>
+      </c>
+      <c r="C93" t="s">
+        <v>132</v>
+      </c>
+      <c r="E93" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="5"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>80</v>
+      </c>
+      <c r="B96" t="s">
+        <v>88</v>
+      </c>
+      <c r="C96" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>81</v>
+      </c>
+      <c r="B97" t="s">
+        <v>88</v>
+      </c>
+      <c r="C97" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>82</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B98" t="s">
         <v>89</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C98" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A73:F73"/>
-    <mergeCell ref="A89:F89"/>
+    <mergeCell ref="A74:F74"/>
+    <mergeCell ref="A95:F95"/>
     <mergeCell ref="H2:J6"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A10:F10"/>
     <mergeCell ref="A20:F20"/>
-    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="A58:F58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2410,10 +2521,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G39" sqref="G38:G39"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2780,69 +2891,80 @@
         <v>181</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>195</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>142</v>
       </c>
-      <c r="B31">
+      <c r="B39">
         <v>3</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F39" s="4" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>141</v>
       </c>
-      <c r="B32">
+      <c r="B40">
         <v>4</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F40" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>139</v>
       </c>
-      <c r="B33">
+      <c r="B41">
         <v>6</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="F41" s="4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>140</v>
       </c>
-      <c r="B34">
+      <c r="B42">
         <v>6</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="F42" s="4" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>191</v>
       </c>
-      <c r="B35">
+      <c r="B43">
         <v>6</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F43" s="4" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>192</v>
       </c>
-      <c r="B36">
+      <c r="B44">
         <v>6</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F44" s="4" t="s">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Dyno System Diagram to Version 2.1 to replace Mid MCN breakout with Dyno MCN breakout Updated Connector Master List to match these changes to Dyno System Diagram Updated all drawings with "MCN backplane" to "MCN breakout", 'cause
</commit_message>
<xml_diff>
--- a/RW-3 Connector Master List.xlsx
+++ b/RW-3 Connector Master List.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="211">
   <si>
     <t>Connector Number</t>
   </si>
@@ -414,12 +414,6 @@
   </si>
   <si>
     <t>Dyno Electrical System Diagram</t>
-  </si>
-  <si>
-    <t>X-4000</t>
-  </si>
-  <si>
-    <t>X-4001</t>
   </si>
   <si>
     <t>X-1000</t>
@@ -679,6 +673,21 @@
   </si>
   <si>
     <t>X-333</t>
+  </si>
+  <si>
+    <t>X-5002</t>
+  </si>
+  <si>
+    <t>X-5003</t>
+  </si>
+  <si>
+    <t>10-crkt MicroClasp</t>
+  </si>
+  <si>
+    <t>C-1006</t>
+  </si>
+  <si>
+    <t>Dyno Flow Sensor &amp; Temp Sensors to Dyno MCN Backplane</t>
   </si>
 </sst>
 </file>
@@ -1246,11 +1255,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J98"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G52" sqref="G52"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,7 +1302,7 @@
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="H2" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="8"/>
@@ -1351,7 +1360,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B6" t="s">
         <v>131</v>
@@ -1360,7 +1369,7 @@
         <v>132</v>
       </c>
       <c r="E6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="13"/>
@@ -1368,7 +1377,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B7" t="s">
         <v>131</v>
@@ -1377,7 +1386,7 @@
         <v>132</v>
       </c>
       <c r="E7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -1385,10 +1394,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C8" t="s">
         <v>132</v>
@@ -1942,7 +1951,7 @@
         <v>43</v>
       </c>
       <c r="B51" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C51" t="s">
         <v>20</v>
@@ -1956,7 +1965,7 @@
         <v>44</v>
       </c>
       <c r="B52" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C52" t="s">
         <v>20</v>
@@ -1967,21 +1976,21 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B53" t="s">
         <v>47</v>
       </c>
       <c r="C53" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E53" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B54" t="s">
         <v>50</v>
@@ -1990,12 +1999,12 @@
         <v>132</v>
       </c>
       <c r="E54" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B55" t="s">
         <v>50</v>
@@ -2004,12 +2013,12 @@
         <v>132</v>
       </c>
       <c r="E55" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B56" t="s">
         <v>50</v>
@@ -2018,7 +2027,7 @@
         <v>132</v>
       </c>
       <c r="E56" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2187,34 +2196,6 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>133</v>
-      </c>
-      <c r="B71" t="s">
-        <v>70</v>
-      </c>
-      <c r="C71" t="s">
-        <v>132</v>
-      </c>
-      <c r="E71" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>134</v>
-      </c>
-      <c r="B72" t="s">
-        <v>70</v>
-      </c>
-      <c r="C72" t="s">
-        <v>132</v>
-      </c>
-      <c r="E72" t="s">
-        <v>142</v>
-      </c>
-    </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>83</v>
@@ -2303,7 +2284,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>119</v>
       </c>
@@ -2314,7 +2295,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>120</v>
       </c>
@@ -2328,7 +2309,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>121</v>
       </c>
@@ -2342,7 +2323,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>122</v>
       </c>
@@ -2353,7 +2334,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>123</v>
       </c>
@@ -2364,7 +2345,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>124</v>
       </c>
@@ -2375,67 +2356,67 @@
         <v>107</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>195</v>
+      </c>
+      <c r="B87" t="s">
+        <v>200</v>
+      </c>
+      <c r="C87" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>196</v>
+      </c>
+      <c r="B88" t="s">
+        <v>200</v>
+      </c>
+      <c r="C88" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>197</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B89" t="s">
+        <v>201</v>
+      </c>
+      <c r="C89" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>198</v>
+      </c>
+      <c r="B90" t="s">
+        <v>201</v>
+      </c>
+      <c r="C90" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>199</v>
+      </c>
+      <c r="B91" t="s">
         <v>202</v>
       </c>
-      <c r="C87" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>198</v>
-      </c>
-      <c r="B88" t="s">
-        <v>202</v>
-      </c>
-      <c r="C88" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>199</v>
-      </c>
-      <c r="B89" t="s">
+      <c r="C91" t="s">
         <v>203</v>
       </c>
-      <c r="C89" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>200</v>
-      </c>
-      <c r="B90" t="s">
-        <v>203</v>
-      </c>
-      <c r="C90" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>201</v>
-      </c>
-      <c r="B91" t="s">
+      <c r="E91" t="s">
         <v>204</v>
       </c>
-      <c r="C91" t="s">
-        <v>205</v>
-      </c>
-      <c r="E91" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B92" t="s">
         <v>86</v>
@@ -2444,12 +2425,12 @@
         <v>132</v>
       </c>
       <c r="E92" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B93" t="s">
         <v>86</v>
@@ -2458,56 +2439,84 @@
         <v>132</v>
       </c>
       <c r="E93" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>206</v>
+      </c>
+      <c r="B94" t="s">
+        <v>208</v>
+      </c>
+      <c r="C94" t="s">
+        <v>132</v>
+      </c>
+      <c r="E94" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>207</v>
+      </c>
+      <c r="B95" t="s">
+        <v>208</v>
+      </c>
+      <c r="C95" t="s">
+        <v>132</v>
+      </c>
+      <c r="E95" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B95" s="5"/>
-      <c r="C95" s="5"/>
-      <c r="D95" s="5"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="5"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>80</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B99" t="s">
         <v>88</v>
       </c>
-      <c r="C96" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="C99" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>81</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B100" t="s">
         <v>88</v>
       </c>
-      <c r="C97" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="C100" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>82</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B101" t="s">
         <v>89</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C101" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A74:F74"/>
-    <mergeCell ref="A95:F95"/>
+    <mergeCell ref="A98:F98"/>
     <mergeCell ref="H2:J6"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A10:F10"/>
@@ -2521,10 +2530,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2542,19 +2551,19 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -2565,10 +2574,10 @@
         <v>5</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I2" s="17"/>
       <c r="J2" s="18"/>
@@ -2581,7 +2590,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H3" s="19"/>
       <c r="I3" s="20"/>
@@ -2595,7 +2604,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H4" s="22"/>
       <c r="I4" s="23"/>
@@ -2609,7 +2618,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2620,7 +2629,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2631,7 +2640,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2642,7 +2651,7 @@
         <v>8</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2653,7 +2662,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2664,7 +2673,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2675,7 +2684,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2686,10 +2695,10 @@
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2700,10 +2709,10 @@
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2714,10 +2723,10 @@
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2728,10 +2737,10 @@
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2742,10 +2751,10 @@
         <v>14</v>
       </c>
       <c r="E16" t="s">
+        <v>164</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2756,7 +2765,7 @@
         <v>6</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2767,7 +2776,7 @@
         <v>6</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2778,7 +2787,7 @@
         <v>6</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2789,7 +2798,7 @@
         <v>6</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2800,7 +2809,7 @@
         <v>6</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2811,7 +2820,7 @@
         <v>6</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2822,7 +2831,7 @@
         <v>6</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2833,7 +2842,7 @@
         <v>6</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2844,18 +2853,18 @@
         <v>6</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B26">
         <v>3</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2866,7 +2875,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2874,10 +2883,10 @@
         <v>127</v>
       </c>
       <c r="B28" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2885,87 +2894,98 @@
         <v>129</v>
       </c>
       <c r="B29" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B30">
         <v>4</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B39">
         <v>3</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B40">
         <v>4</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B41">
         <v>6</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B42">
         <v>6</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B43">
         <v>6</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B44">
         <v>6</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>209</v>
+      </c>
+      <c r="B45">
+        <v>9</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed pinouts for M12s to match the wiki
</commit_message>
<xml_diff>
--- a/RW-3 Connector Master List.xlsx
+++ b/RW-3 Connector Master List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="1" r:id="rId1"/>
@@ -1257,7 +1257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D90" sqref="D90"/>
     </sheetView>
@@ -2532,8 +2532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2916,7 +2916,7 @@
         <v>140</v>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>182</v>

</xml_diff>

<commit_message>
Created Rear Enclosure Diagram Version 1.0 Updated RW-3 Electrical System Diagram to Version 1.2 Updated RW-3 Connector Master List for Rear Enclosure connectors
</commit_message>
<xml_diff>
--- a/RW-3 Connector Master List.xlsx
+++ b/RW-3 Connector Master List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="231">
   <si>
     <t>Connector Number</t>
   </si>
@@ -150,9 +150,6 @@
   </si>
   <si>
     <t>X-332</t>
-  </si>
-  <si>
-    <t>2-crkt Micro-Fit</t>
   </si>
   <si>
     <t>C-102</t>
@@ -688,6 +685,69 @@
   </si>
   <si>
     <t>Dyno Flow Sensor &amp; Temp Sensors to Dyno MCN Backplane</t>
+  </si>
+  <si>
+    <t>X-334</t>
+  </si>
+  <si>
+    <t>2-crkt Micro-Fit DR</t>
+  </si>
+  <si>
+    <t>2-crkt Micro-Fit SR</t>
+  </si>
+  <si>
+    <t>X-103</t>
+  </si>
+  <si>
+    <t>Ext_+12V from X-103 to DC-DC Converter</t>
+  </si>
+  <si>
+    <t>C-130</t>
+  </si>
+  <si>
+    <t>C-131</t>
+  </si>
+  <si>
+    <t>C-132</t>
+  </si>
+  <si>
+    <t>DC-DC On/Off switch to DC-DC Converter</t>
+  </si>
+  <si>
+    <t>DC-DC Converter Sensor Signals to Rear MCN</t>
+  </si>
+  <si>
+    <t>+12V to Rear CAN Backplane</t>
+  </si>
+  <si>
+    <t>X-335</t>
+  </si>
+  <si>
+    <t>X-336</t>
+  </si>
+  <si>
+    <t>X-337</t>
+  </si>
+  <si>
+    <t>X-517</t>
+  </si>
+  <si>
+    <t>X-338</t>
+  </si>
+  <si>
+    <t>X-339</t>
+  </si>
+  <si>
+    <t>X-340</t>
+  </si>
+  <si>
+    <t>C-133</t>
+  </si>
+  <si>
+    <t>CAN 2 from Rear MCN to Rear MCN Backplane</t>
+  </si>
+  <si>
+    <t>X-413</t>
   </si>
 </sst>
 </file>
@@ -885,12 +945,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -950,6 +1004,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1255,11 +1315,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J101"/>
+  <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D90" sqref="D90"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,19 +1353,19 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="H2" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="8"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="H2" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1320,9 +1380,9 @@
       <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="11"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1337,9 +1397,9 @@
       <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="11"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1354,85 +1414,88 @@
       <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="11"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>213</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>187</v>
       </c>
       <c r="C6" t="s">
-        <v>132</v>
+        <v>202</v>
       </c>
       <c r="E6" t="s">
-        <v>139</v>
-      </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="14"/>
+        <v>203</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>186</v>
+        <v>132</v>
       </c>
       <c r="B7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" t="s">
         <v>131</v>
       </c>
-      <c r="C7" t="s">
-        <v>132</v>
-      </c>
       <c r="E7" t="s">
-        <v>139</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+        <v>138</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B8" t="s">
-        <v>188</v>
+        <v>130</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>131</v>
+      </c>
+      <c r="E8" t="s">
+        <v>138</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C9" t="s">
+        <v>131</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" t="s">
-        <v>23</v>
-      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -1446,7 +1509,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
@@ -1455,40 +1518,40 @@
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>26</v>
@@ -1496,10 +1559,13 @@
       <c r="C16" t="s">
         <v>20</v>
       </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>26</v>
@@ -1507,13 +1573,10 @@
       <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="E17" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
@@ -1521,37 +1584,37 @@
       <c r="C18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="E18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" t="s">
-        <v>22</v>
-      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>211</v>
       </c>
       <c r="C22" t="s">
         <v>20</v>
@@ -1562,966 +1625,1094 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>211</v>
       </c>
       <c r="C23" t="s">
         <v>20</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
         <v>20</v>
       </c>
       <c r="E24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" t="s">
         <v>45</v>
-      </c>
-      <c r="C25" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
+        <v>211</v>
+      </c>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" t="s">
         <v>47</v>
-      </c>
-      <c r="C26" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
         <v>20</v>
       </c>
       <c r="E27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>211</v>
       </c>
       <c r="C28" t="s">
         <v>20</v>
       </c>
       <c r="E28" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
         <v>20</v>
       </c>
       <c r="E29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>211</v>
       </c>
       <c r="C30" t="s">
         <v>20</v>
       </c>
       <c r="E30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C31" t="s">
         <v>20</v>
       </c>
       <c r="E31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C32" t="s">
         <v>20</v>
       </c>
       <c r="E32" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>90</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="E33" t="s">
-        <v>108</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B34" t="s">
-        <v>50</v>
+        <v>212</v>
       </c>
       <c r="C34" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34" t="s">
         <v>107</v>
-      </c>
-      <c r="E34" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E36" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E37" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E38" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E40" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E41" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E42" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E43" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E44" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E45" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E46" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E47" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>103</v>
+      </c>
+      <c r="B48" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" t="s">
+        <v>106</v>
+      </c>
+      <c r="E48" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>104</v>
+      </c>
+      <c r="B49" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" t="s">
+        <v>106</v>
+      </c>
+      <c r="E49" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>105</v>
       </c>
-      <c r="B48" t="s">
-        <v>50</v>
-      </c>
-      <c r="C48" t="s">
-        <v>107</v>
-      </c>
-      <c r="E48" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="B50" t="s">
+        <v>212</v>
+      </c>
+      <c r="C50" t="s">
         <v>106</v>
       </c>
-      <c r="B49" t="s">
-        <v>45</v>
-      </c>
-      <c r="C49" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>42</v>
       </c>
-      <c r="B50" t="s">
-        <v>50</v>
-      </c>
-      <c r="C50" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>43</v>
       </c>
-      <c r="B51" t="s">
-        <v>167</v>
-      </c>
-      <c r="C51" t="s">
-        <v>20</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="B52" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53" t="s">
+        <v>166</v>
+      </c>
+      <c r="C53" t="s">
+        <v>20</v>
+      </c>
+      <c r="E53" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>204</v>
+      </c>
+      <c r="B54" t="s">
+        <v>46</v>
+      </c>
+      <c r="C54" t="s">
+        <v>202</v>
+      </c>
+      <c r="E54" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>210</v>
+      </c>
+      <c r="B55" t="s">
+        <v>212</v>
+      </c>
+      <c r="C55" t="s">
+        <v>202</v>
+      </c>
+      <c r="E55" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>221</v>
+      </c>
+      <c r="B56" t="s">
+        <v>46</v>
+      </c>
+      <c r="C56" t="s">
+        <v>202</v>
+      </c>
+      <c r="E56" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>222</v>
+      </c>
+      <c r="B57" t="s">
+        <v>46</v>
+      </c>
+      <c r="C57" t="s">
+        <v>202</v>
+      </c>
+      <c r="E57" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>223</v>
+      </c>
+      <c r="B58" t="s">
+        <v>46</v>
+      </c>
+      <c r="C58" t="s">
+        <v>202</v>
+      </c>
+      <c r="E58" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>225</v>
+      </c>
+      <c r="B59" t="s">
+        <v>49</v>
+      </c>
+      <c r="C59" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>226</v>
+      </c>
+      <c r="B60" t="s">
+        <v>49</v>
+      </c>
+      <c r="C60" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>227</v>
+      </c>
+      <c r="B61" t="s">
+        <v>212</v>
+      </c>
+      <c r="C61" t="s">
+        <v>202</v>
+      </c>
+      <c r="E61" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>133</v>
+      </c>
+      <c r="B62" t="s">
+        <v>49</v>
+      </c>
+      <c r="C62" t="s">
+        <v>131</v>
+      </c>
+      <c r="E62" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>134</v>
+      </c>
+      <c r="B63" t="s">
+        <v>49</v>
+      </c>
+      <c r="C63" t="s">
+        <v>131</v>
+      </c>
+      <c r="E63" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>135</v>
+      </c>
+      <c r="B64" t="s">
+        <v>49</v>
+      </c>
+      <c r="C64" t="s">
+        <v>131</v>
+      </c>
+      <c r="E64" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>44</v>
-      </c>
-      <c r="B52" t="s">
-        <v>167</v>
-      </c>
-      <c r="C52" t="s">
-        <v>20</v>
-      </c>
-      <c r="E52" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>205</v>
-      </c>
-      <c r="B53" t="s">
-        <v>47</v>
-      </c>
-      <c r="C53" t="s">
-        <v>203</v>
-      </c>
-      <c r="E53" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>134</v>
-      </c>
-      <c r="B54" t="s">
-        <v>50</v>
-      </c>
-      <c r="C54" t="s">
-        <v>132</v>
-      </c>
-      <c r="E54" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>135</v>
-      </c>
-      <c r="B55" t="s">
-        <v>50</v>
-      </c>
-      <c r="C55" t="s">
-        <v>132</v>
-      </c>
-      <c r="E55" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>136</v>
-      </c>
-      <c r="B56" t="s">
-        <v>50</v>
-      </c>
-      <c r="C56" t="s">
-        <v>132</v>
-      </c>
-      <c r="E56" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>56</v>
-      </c>
-      <c r="B59" t="s">
-        <v>68</v>
-      </c>
-      <c r="C59" t="s">
-        <v>20</v>
-      </c>
-      <c r="E59" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>57</v>
-      </c>
-      <c r="B60" t="s">
-        <v>68</v>
-      </c>
-      <c r="C60" t="s">
-        <v>20</v>
-      </c>
-      <c r="E60" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>58</v>
-      </c>
-      <c r="B61" t="s">
-        <v>69</v>
-      </c>
-      <c r="C61" t="s">
-        <v>20</v>
-      </c>
-      <c r="E61" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>59</v>
-      </c>
-      <c r="B62" t="s">
-        <v>68</v>
-      </c>
-      <c r="C62" t="s">
-        <v>20</v>
-      </c>
-      <c r="E62" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>60</v>
-      </c>
-      <c r="B63" t="s">
-        <v>68</v>
-      </c>
-      <c r="C63" t="s">
-        <v>20</v>
-      </c>
-      <c r="E63" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>61</v>
-      </c>
-      <c r="B64" t="s">
-        <v>69</v>
-      </c>
-      <c r="C64" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>62</v>
-      </c>
-      <c r="B65" t="s">
-        <v>69</v>
-      </c>
-      <c r="C65" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>63</v>
-      </c>
-      <c r="B66" t="s">
-        <v>70</v>
-      </c>
-      <c r="C66" t="s">
-        <v>20</v>
-      </c>
-      <c r="E66" t="s">
-        <v>72</v>
-      </c>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B67" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C67" t="s">
         <v>20</v>
       </c>
       <c r="E67" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B68" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C68" t="s">
         <v>20</v>
       </c>
       <c r="E68" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B69" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C69" t="s">
         <v>20</v>
+      </c>
+      <c r="E69" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B70" t="s">
         <v>67</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
+        <v>20</v>
+      </c>
+      <c r="E70" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>59</v>
+      </c>
+      <c r="B71" t="s">
+        <v>67</v>
+      </c>
+      <c r="C71" t="s">
+        <v>20</v>
+      </c>
+      <c r="E71" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>60</v>
+      </c>
+      <c r="B72" t="s">
+        <v>68</v>
+      </c>
+      <c r="C72" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>61</v>
+      </c>
+      <c r="B73" t="s">
+        <v>68</v>
+      </c>
+      <c r="C73" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>62</v>
+      </c>
+      <c r="B74" t="s">
+        <v>69</v>
+      </c>
+      <c r="C74" t="s">
+        <v>20</v>
+      </c>
+      <c r="E74" t="s">
         <v>71</v>
       </c>
-      <c r="C70" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B75" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C75" t="s">
         <v>20</v>
       </c>
       <c r="E75" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B76" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C76" t="s">
         <v>20</v>
       </c>
       <c r="E76" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B77" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="C77" t="s">
         <v>20</v>
-      </c>
-      <c r="E77" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B78" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C78" t="s">
         <v>20</v>
-      </c>
-      <c r="E78" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>230</v>
       </c>
       <c r="B79" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="C79" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>73</v>
+      </c>
+      <c r="B83" t="s">
+        <v>83</v>
+      </c>
+      <c r="C83" t="s">
+        <v>20</v>
+      </c>
+      <c r="E83" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>74</v>
+      </c>
+      <c r="B84" t="s">
+        <v>84</v>
+      </c>
+      <c r="C84" t="s">
+        <v>20</v>
+      </c>
+      <c r="E84" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>75</v>
+      </c>
+      <c r="B85" t="s">
+        <v>85</v>
+      </c>
+      <c r="C85" t="s">
+        <v>20</v>
+      </c>
+      <c r="E85" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>76</v>
+      </c>
+      <c r="B86" t="s">
+        <v>85</v>
+      </c>
+      <c r="C86" t="s">
+        <v>20</v>
+      </c>
+      <c r="E86" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>77</v>
+      </c>
+      <c r="B87" t="s">
+        <v>86</v>
+      </c>
+      <c r="C87" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>117</v>
+      </c>
+      <c r="B88" t="s">
+        <v>124</v>
+      </c>
+      <c r="C88" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>118</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B89" t="s">
+        <v>124</v>
+      </c>
+      <c r="C89" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>119</v>
+      </c>
+      <c r="B90" t="s">
         <v>125</v>
       </c>
-      <c r="C80" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>119</v>
-      </c>
-      <c r="B81" t="s">
-        <v>125</v>
-      </c>
-      <c r="C81" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="C90" t="s">
+        <v>106</v>
+      </c>
+      <c r="E90" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>120</v>
       </c>
-      <c r="B82" t="s">
-        <v>126</v>
-      </c>
-      <c r="C82" t="s">
-        <v>107</v>
-      </c>
-      <c r="E82" t="s">
+      <c r="B91" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="C91" t="s">
+        <v>106</v>
+      </c>
+      <c r="E91" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>121</v>
       </c>
-      <c r="B83" t="s">
-        <v>128</v>
-      </c>
-      <c r="C83" t="s">
-        <v>107</v>
-      </c>
-      <c r="E83" t="s">
+      <c r="B92" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="C92" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>122</v>
       </c>
-      <c r="B84" t="s">
-        <v>130</v>
-      </c>
-      <c r="C84" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="B93" t="s">
+        <v>129</v>
+      </c>
+      <c r="C93" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>123</v>
       </c>
-      <c r="B85" t="s">
-        <v>130</v>
-      </c>
-      <c r="C85" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>124</v>
-      </c>
-      <c r="B86" t="s">
-        <v>130</v>
-      </c>
-      <c r="C86" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="B94" t="s">
+        <v>129</v>
+      </c>
+      <c r="C94" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>194</v>
+      </c>
+      <c r="B95" t="s">
+        <v>199</v>
+      </c>
+      <c r="C95" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>195</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B96" t="s">
+        <v>199</v>
+      </c>
+      <c r="C96" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>196</v>
+      </c>
+      <c r="B97" t="s">
         <v>200</v>
       </c>
-      <c r="C87" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>196</v>
-      </c>
-      <c r="B88" t="s">
+      <c r="C97" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>197</v>
+      </c>
+      <c r="B98" t="s">
         <v>200</v>
       </c>
-      <c r="C88" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>197</v>
-      </c>
-      <c r="B89" t="s">
-        <v>201</v>
-      </c>
-      <c r="C89" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>198</v>
-      </c>
-      <c r="B90" t="s">
-        <v>201</v>
-      </c>
-      <c r="C90" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>199</v>
-      </c>
-      <c r="B91" t="s">
+      <c r="C98" t="s">
         <v>202</v>
       </c>
-      <c r="C91" t="s">
-        <v>203</v>
-      </c>
-      <c r="E91" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>142</v>
-      </c>
-      <c r="B92" t="s">
-        <v>86</v>
-      </c>
-      <c r="C92" t="s">
-        <v>132</v>
-      </c>
-      <c r="E92" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>141</v>
-      </c>
-      <c r="B93" t="s">
-        <v>86</v>
-      </c>
-      <c r="C93" t="s">
-        <v>132</v>
-      </c>
-      <c r="E93" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>206</v>
-      </c>
-      <c r="B94" t="s">
-        <v>208</v>
-      </c>
-      <c r="C94" t="s">
-        <v>132</v>
-      </c>
-      <c r="E94" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>207</v>
-      </c>
-      <c r="B95" t="s">
-        <v>208</v>
-      </c>
-      <c r="C95" t="s">
-        <v>132</v>
-      </c>
-      <c r="E95" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B98" s="5"/>
-      <c r="C98" s="5"/>
-      <c r="D98" s="5"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="5"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>80</v>
+        <v>198</v>
       </c>
       <c r="B99" t="s">
-        <v>88</v>
+        <v>201</v>
       </c>
       <c r="C99" t="s">
-        <v>20</v>
+        <v>202</v>
+      </c>
+      <c r="E99" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>224</v>
+      </c>
+      <c r="B100" t="s">
+        <v>129</v>
+      </c>
+      <c r="C100" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>141</v>
+      </c>
+      <c r="B102" t="s">
+        <v>85</v>
+      </c>
+      <c r="C102" t="s">
+        <v>131</v>
+      </c>
+      <c r="E102" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>140</v>
+      </c>
+      <c r="B103" t="s">
+        <v>85</v>
+      </c>
+      <c r="C103" t="s">
+        <v>131</v>
+      </c>
+      <c r="E103" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>205</v>
+      </c>
+      <c r="B104" t="s">
+        <v>207</v>
+      </c>
+      <c r="C104" t="s">
+        <v>131</v>
+      </c>
+      <c r="E104" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>206</v>
+      </c>
+      <c r="B105" t="s">
+        <v>207</v>
+      </c>
+      <c r="C105" t="s">
+        <v>131</v>
+      </c>
+      <c r="E105" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B108" s="3"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="3"/>
+      <c r="F108" s="3"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>79</v>
+      </c>
+      <c r="B109" t="s">
+        <v>87</v>
+      </c>
+      <c r="C109" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>80</v>
+      </c>
+      <c r="B110" t="s">
+        <v>87</v>
+      </c>
+      <c r="C110" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>81</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B111" t="s">
         <v>88</v>
       </c>
-      <c r="C100" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>82</v>
-      </c>
-      <c r="B101" t="s">
-        <v>89</v>
-      </c>
-      <c r="C101" t="s">
+      <c r="C111" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A74:F74"/>
-    <mergeCell ref="A98:F98"/>
-    <mergeCell ref="H2:J6"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A108:F108"/>
+    <mergeCell ref="H2:J7"/>
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="A58:F58"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A66:F66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2532,8 +2723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I39" sqref="I37:I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2543,7 +2734,7 @@
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20" style="4" customWidth="1"/>
+    <col min="6" max="6" width="20" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2551,19 +2742,19 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="23" t="s">
         <v>148</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -2573,14 +2764,14 @@
       <c r="B2">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
+      <c r="F2" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2" s="15"/>
+      <c r="J2" s="16"/>
     </row>
     <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2589,102 +2780,102 @@
       <c r="B3">
         <v>6</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="21"/>
+      <c r="F3" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4">
         <v>6</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="H4" s="22"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="24"/>
+      <c r="F4" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="H4" s="20"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="22"/>
     </row>
     <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5">
         <v>8</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>154</v>
+      <c r="F5" s="24" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>155</v>
+      <c r="F6" s="24" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>7</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>156</v>
+      <c r="F7" s="24" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>8</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>157</v>
+      <c r="F8" s="24" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>158</v>
+      <c r="F9" s="24" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>159</v>
+      <c r="F10" s="24" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>160</v>
+      <c r="F11" s="24" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2695,10 +2886,10 @@
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>164</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>161</v>
+        <v>163</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2709,10 +2900,10 @@
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>164</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>162</v>
+        <v>163</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2723,10 +2914,10 @@
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>164</v>
-      </c>
-      <c r="F14" s="4" t="s">
         <v>163</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2737,255 +2928,310 @@
         <v>6</v>
       </c>
       <c r="E15" t="s">
+        <v>163</v>
+      </c>
+      <c r="F15" s="24" t="s">
         <v>164</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16">
         <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>164</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B17">
         <v>6</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>168</v>
+      <c r="F17" s="24" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B18">
         <v>6</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>169</v>
+      <c r="F18" s="24" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B19">
         <v>6</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>170</v>
+      <c r="F19" s="24" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B20">
         <v>6</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>171</v>
+      <c r="F20" s="24" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B21">
         <v>6</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>172</v>
+      <c r="F21" s="24" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B22">
         <v>6</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>173</v>
+      <c r="F22" s="24" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B23">
         <v>6</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>174</v>
+      <c r="F23" s="24" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B24">
         <v>6</v>
       </c>
-      <c r="F24" s="4" t="s">
-        <v>181</v>
+      <c r="F24" s="24" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B25">
         <v>6</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>175</v>
+      <c r="F25" s="24" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B26">
         <v>3</v>
       </c>
-      <c r="F26" s="4" t="s">
-        <v>176</v>
+      <c r="F26" s="24" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>177</v>
+      <c r="F27" s="24" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B28" t="s">
-        <v>180</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>178</v>
+        <v>179</v>
+      </c>
+      <c r="F28" s="24" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B29" t="s">
-        <v>180</v>
-      </c>
-      <c r="F29" s="4" t="s">
         <v>179</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B30">
         <v>4</v>
       </c>
-      <c r="F30" s="4" t="s">
-        <v>194</v>
+      <c r="F30" s="24" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>203</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>215</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="F32" s="24" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>216</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="F33" s="24" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>217</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="F34" s="24" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>228</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B39">
         <v>6</v>
       </c>
-      <c r="F39" s="4" t="s">
-        <v>182</v>
+      <c r="F39" s="24" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B40">
         <v>4</v>
       </c>
-      <c r="F40" s="4" t="s">
-        <v>183</v>
+      <c r="F40" s="24" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B41">
         <v>6</v>
       </c>
-      <c r="F41" s="4" t="s">
-        <v>184</v>
+      <c r="F41" s="24" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B42">
         <v>6</v>
       </c>
-      <c r="F42" s="4" t="s">
-        <v>185</v>
+      <c r="F42" s="24" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B43">
         <v>6</v>
       </c>
-      <c r="F43" s="4" t="s">
-        <v>192</v>
+      <c r="F43" s="24" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B44">
         <v>6</v>
       </c>
-      <c r="F44" s="4" t="s">
-        <v>191</v>
+      <c r="F44" s="24" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B45">
         <v>9</v>
       </c>
-      <c r="F45" s="4" t="s">
-        <v>210</v>
+      <c r="F45" s="24" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2993,5 +3239,6 @@
     <mergeCell ref="H2:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>